<commit_message>
Update to Unity2018 Fix Example
</commit_message>
<xml_diff>
--- a/Documents/TagReference.xlsx
+++ b/Documents/TagReference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izutsu\Desktop\Trionfi\Assets\Trionfi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\井筒　紗奈\Desktop\Trionfi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635032D2-DBAC-4E52-9296-3CB59B2BD045}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D811428A-0673-48AB-B311-90C8E17C9ACC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{7F702E2A-9EB7-4142-98AC-0C9039DFE745}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{7F702E2A-9EB7-4142-98AC-0C9039DFE745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="153">
   <si>
     <t>タグ名</t>
     <rPh sb="2" eb="3">
@@ -806,43 +806,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>videoplay</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>動画のパスorURL</t>
-    <rPh sb="0" eb="2">
-      <t>ドウガ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ローカルの場合はAssets/からの相対パス。</t>
-    <rPh sb="5" eb="7">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ソウタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>loop</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ループさせる</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>動画の一時停止</t>
     <rPh sb="0" eb="2">
       <t>ドウガ</t>
@@ -988,6 +951,156 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t>ヒンド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキストレイヤに文字を表示する</t>
+    <rPh sb="8" eb="10">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>laytext</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>動機</t>
+    <rPh sb="0" eb="2">
+      <t>ドウキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表示する文字列</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>モジレツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>actor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レイヤに紐付けるキャラ名（messageの話者と関連します）</t>
+    <rPh sb="4" eb="6">
+      <t>ヒモヅ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ワシャ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>カンレン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>snap</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レイヤのサイズを画像のサイズにあわせる</t>
+    <rPh sb="8" eb="10">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>width</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>height</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画面幅</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ハバ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画面高さ</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レイヤのwidthを指定（snapとは排他）</t>
+    <rPh sb="10" eb="12">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ハイタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レイヤのheightを指定（snapとは排他）</t>
+    <rPh sb="11" eb="13">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ハイタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mesface</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>台詞ウィンドウの画像指定</t>
+    <rPh sb="0" eb="2">
+      <t>セリフ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画像ファイル名</t>
+    <rPh sb="0" eb="2">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メッセージウィンドウと一体化している場合は不要</t>
+    <rPh sb="11" eb="14">
+      <t>イッタイカ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>フヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1356,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A7694E-C34A-4AF6-AD55-184CC16CE10F}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1626,394 +1739,400 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D18" t="s">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>49</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>50</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D21" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E22" t="s">
         <v>20</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D19" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D23" t="s">
         <v>19</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E23" t="s">
         <v>23</v>
       </c>
-      <c r="F19">
+      <c r="F23">
         <v>0</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G23" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
         <v>69</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
         <v>73</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>74</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>1000</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D25" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D26" t="s">
         <v>76</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>77</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>78</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
         <v>79</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I26" t="s">
-        <v>119</v>
-      </c>
-    </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" t="s">
+        <v>137</v>
+      </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="E27" t="s">
-        <v>121</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>33</v>
       </c>
       <c r="G27" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>131</v>
-      </c>
-      <c r="E31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" t="s">
-        <v>138</v>
-      </c>
-      <c r="I31" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
-      <c r="D32" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32">
-        <v>5</v>
-      </c>
-      <c r="G32" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D33" t="s">
-        <v>140</v>
-      </c>
-      <c r="E33" t="s">
-        <v>137</v>
-      </c>
-      <c r="F33">
-        <v>20</v>
-      </c>
-      <c r="G33" t="s">
-        <v>141</v>
+      <c r="A33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
+      <c r="D34" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" t="s">
+        <v>131</v>
+      </c>
+      <c r="I34" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" t="s">
-        <v>85</v>
+      <c r="D36" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+      <c r="G36" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G37" t="s">
-        <v>92</v>
+        <v>151</v>
+      </c>
+      <c r="I37" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D38" t="s">
-        <v>93</v>
-      </c>
-      <c r="E38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F38" t="s">
-        <v>94</v>
-      </c>
-      <c r="G38" t="s">
-        <v>95</v>
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
         <v>85</v>
@@ -2021,33 +2140,27 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
         <v>85</v>
       </c>
-      <c r="D40" t="s">
-        <v>99</v>
-      </c>
-      <c r="E40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F40" t="s">
-        <v>94</v>
-      </c>
-      <c r="G40" t="s">
-        <v>102</v>
-      </c>
-      <c r="I40" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E41" t="s">
         <v>91</v>
@@ -2056,21 +2169,12 @@
         <v>94</v>
       </c>
       <c r="G41" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
-      </c>
       <c r="D42" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E42" t="s">
         <v>91</v>
@@ -2079,32 +2183,32 @@
         <v>94</v>
       </c>
       <c r="G42" t="s">
-        <v>108</v>
-      </c>
-      <c r="I42" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
         <v>85</v>
       </c>
-      <c r="I43" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
       </c>
       <c r="D44" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E44" t="s">
         <v>91</v>
@@ -2113,17 +2217,91 @@
         <v>94</v>
       </c>
       <c r="G44" t="s">
+        <v>102</v>
+      </c>
+      <c r="I44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D45" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" t="s">
+        <v>94</v>
+      </c>
+      <c r="G45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" t="s">
+        <v>107</v>
+      </c>
+      <c r="E46" t="s">
+        <v>91</v>
+      </c>
+      <c r="F46" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" t="s">
         <v>108</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="I47" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" t="s">
+        <v>94</v>
+      </c>
+      <c r="G48" t="s">
+        <v>108</v>
+      </c>
+      <c r="I48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>113</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I49" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>